<commit_message>
dif energy values for seq and pipeline
</commit_message>
<xml_diff>
--- a/workspace/notebook/convPePipelineVsSequentialGraph.xlsx
+++ b/workspace/notebook/convPePipelineVsSequentialGraph.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\macse\Downloads\6.5930\6.5930FinalProject\workspace\notebook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{750D842C-44E7-45AA-8BF1-CD617E3BD22F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57CA20AE-4F0D-489A-8156-DD153C296D29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{CB355DDA-E86D-4EF4-B8A2-C4314606351C}"/>
   </bookViews>
@@ -672,538 +672,6 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Total</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> E</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>nergy over PE Size (Pipeline)</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:scatterChart>
-        <c:scatterStyle val="smoothMarker"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>peTestSequentialConv!$F$24</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>total_energy (Pipeline)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>peTestSequentialConv!$A$25:$A$40</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="16"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>16</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>peTestSequentialConv!$F$25:$F$40</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="16"/>
-                <c:pt idx="0">
-                  <c:v>450206462512817.75</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>900476557864701.5</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>900731088931686.5</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>901112986303237.5</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>901622249352922.5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>902322409546239.5</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>903149835501977.5</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>903977257457715.5</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>905059316938296.5</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>907096174137036.5</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>908432864142459.5</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>912506556539939.5</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>916580248937419.5</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>916580248937419.5</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>916580248937419.5</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>916580248937419.5</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="1"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-7C6A-4CBD-AECA-DF9950E1A155}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="492507056"/>
-        <c:axId val="492518096"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="492507056"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>PE Size</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="492518096"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="492518096"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Tota</a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr lang="en-US" baseline="0"/>
-                  <a:t>l Energy</a:t>
-                </a:r>
-                <a:endParaRPr lang="en-US"/>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="492507056"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
               <a:t>Intermediate Buffer Energy Over PE Shape (Pipeline)</a:t>
             </a:r>
           </a:p>
@@ -1638,533 +1106,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:sysClr val="windowText" lastClr="000000">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:sysClr>
-                </a:solidFill>
-              </a:rPr>
-              <a:t>Total Energy over PE Size (Sequential)</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:scatterChart>
-        <c:scatterStyle val="smoothMarker"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>peTestSequentialConv!$G$24</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>total_energy (Sequential)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>peTestSequentialConv!$A$25:$A$40</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="16"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>16</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>peTestSequentialConv!$G$25:$G$40</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="16"/>
-                <c:pt idx="0">
-                  <c:v>450261322512817.75</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>450324292351883.75</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>450514714579802.75</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>450705931723434.75</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>451025293629487.75</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>451406727916751.75</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>451851234585225.75</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>452231668872489.75</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>452933465065806.75</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>454274985071229.75</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>454274985071229.75</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>458339617468709.75</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>458339617468709.75</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>458339617468709.75</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>458339617468709.75</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>458339617468709.75</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="1"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-59AC-42A4-8A4B-59523B3687F0}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="572053952"/>
-        <c:axId val="572050592"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="572053952"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>PE Size</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="572050592"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="572050592"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Total Energy</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="572053952"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -2580,7 +1522,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -3277,6 +2219,1060 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Total</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Energy over PE Size </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>(Pipeline)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>peTestSequentialConv!$F$24</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>total_energy (Pipeline)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>peTestSequentialConv!$A$25:$A$40</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>peTestSequentialConv!$F$25:$F$40</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>450206521661981.44</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>450270172696404.06</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>450461125799672</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>450652078902939.94</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>450970334075053.06</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>451352240281588.94</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>451797797522547.44</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>452179703729083.31</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>452879865107732.38</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>454216536830607.81</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>454216536830607.81</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>458290203033656.69</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>458290203033656.69</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>458290203033656.69</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>458290203033656.69</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>458290203033656.69</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-B477-460C-80D9-E04CE2E5C7AC}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1007416111"/>
+        <c:axId val="1007416591"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1007416111"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>PE Size</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1007416591"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1007416591"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Energy</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1007416111"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Total</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Energy over PE Size</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t> (Sequential)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>peTestSequentialConv!$G$24</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>total_energy (Sequential)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>peTestSequentialConv!$A$25:$A$40</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>peTestSequentialConv!$G$25:$G$40</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>517844706826781.38</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>518037990968762.44</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>518617843394705.56</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>519197695820648.69</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>520164116530553.81</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>521323821382440.13</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>522676810376307.44</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>523836515228193.69</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>525962640789985.13</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>530021607771586.94</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>530021607771586.94</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>542391792858373.44</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>542391792858373.44</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>542391792858373.44</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>542391792858373.44</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>542391792858373.44</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-F5E1-49B7-BB73-4A9BDF005540}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1009637375"/>
+        <c:axId val="1009638335"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1009637375"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>PE Size</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1009638335"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1009638335"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Energy</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1009637375"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -6061,42 +6057,6 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>447675</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>15875</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>511175</xdr:colOff>
-      <xdr:row>55</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1FD15E18-9356-6721-6846-F990632C1AB2}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>720724</xdr:colOff>
       <xdr:row>41</xdr:row>
@@ -6125,43 +6085,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>441325</xdr:colOff>
-      <xdr:row>57</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>504825</xdr:colOff>
-      <xdr:row>72</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="5" name="Chart 4">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C8564A07-DE8E-F24D-7755-332C36753208}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -6197,7 +6121,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -6222,6 +6146,78 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3D6ADB50-DF85-BCAF-D535-416BEB7040A4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>79375</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>320675</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>60325</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CC595B58-69D2-8259-3ED3-7ECCF65DBAA9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>365125</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>428625</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>174625</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="8" name="Chart 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4FFE14EE-D4D4-2DF9-5914-D50A4114C5DA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6561,8 +6557,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{834218F4-790A-4AA4-9545-A60C5B12B8E6}">
   <dimension ref="A1:M40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="F58" sqref="F58"/>
+    <sheetView tabSelected="1" topLeftCell="E25" workbookViewId="0">
+      <selection activeCell="T10" sqref="T10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7312,10 +7308,10 @@
         <v>30897457857</v>
       </c>
       <c r="F25">
-        <v>450206462512817.75</v>
+        <v>450206521661981.44</v>
       </c>
       <c r="G25">
-        <v>450261322512817.75</v>
+        <v>517844706826781.38</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.35">
@@ -7335,10 +7331,10 @@
         <v>61794915713</v>
       </c>
       <c r="F26">
-        <v>900476557864701.5</v>
+        <v>450270172696404.06</v>
       </c>
       <c r="G26">
-        <v>450324292351883.75</v>
+        <v>518037990968762.44</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.35">
@@ -7358,10 +7354,10 @@
         <v>154487000000</v>
       </c>
       <c r="F27">
-        <v>900731088931686.5</v>
+        <v>450461125799672</v>
       </c>
       <c r="G27">
-        <v>450514714579802.75</v>
+        <v>518617843394705.56</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.35">
@@ -7381,10 +7377,10 @@
         <v>247180000000</v>
       </c>
       <c r="F28">
-        <v>901112986303237.5</v>
+        <v>450652078902939.94</v>
       </c>
       <c r="G28">
-        <v>450705931723434.75</v>
+        <v>519197695820648.69</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.35">
@@ -7404,10 +7400,10 @@
         <v>401667000000</v>
       </c>
       <c r="F29">
-        <v>901622249352922.5</v>
+        <v>450970334075053.06</v>
       </c>
       <c r="G29">
-        <v>451025293629487.75</v>
+        <v>520164116530553.81</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.35">
@@ -7427,10 +7423,10 @@
         <v>587052000000</v>
       </c>
       <c r="F30">
-        <v>902322409546239.5</v>
+        <v>451352240281588.94</v>
       </c>
       <c r="G30">
-        <v>451406727916751.75</v>
+        <v>521323821382440.13</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.35">
@@ -7450,10 +7446,10 @@
         <v>803334000000</v>
       </c>
       <c r="F31">
-        <v>903149835501977.5</v>
+        <v>451797797522547.44</v>
       </c>
       <c r="G31">
-        <v>451851234585225.75</v>
+        <v>522676810376307.44</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.35">
@@ -7473,10 +7469,10 @@
         <v>988719000000</v>
       </c>
       <c r="F32">
-        <v>903977257457715.5</v>
+        <v>452179703729083.31</v>
       </c>
       <c r="G32">
-        <v>452231668872489.75</v>
+        <v>523836515228193.69</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.35">
@@ -7496,10 +7492,10 @@
         <v>1328590000000</v>
       </c>
       <c r="F33">
-        <v>905059316938296.5</v>
+        <v>452879865107732.38</v>
       </c>
       <c r="G33">
-        <v>452933465065806.75</v>
+        <v>525962640789985.13</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.35">
@@ -7519,10 +7515,10 @@
         <v>1977440000000</v>
       </c>
       <c r="F34">
-        <v>907096174137036.5</v>
+        <v>454216536830607.81</v>
       </c>
       <c r="G34">
-        <v>454274985071229.75</v>
+        <v>530021607771586.94</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.35">
@@ -7542,10 +7538,10 @@
         <v>1977440000000</v>
       </c>
       <c r="F35">
-        <v>908432864142459.5</v>
+        <v>454216536830607.81</v>
       </c>
       <c r="G35">
-        <v>454274985071229.75</v>
+        <v>530021607771586.94</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.35">
@@ -7565,10 +7561,10 @@
         <v>3954870000000</v>
       </c>
       <c r="F36">
-        <v>912506556539939.5</v>
+        <v>458290203033656.69</v>
       </c>
       <c r="G36">
-        <v>458339617468709.75</v>
+        <v>542391792858373.44</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.35">
@@ -7588,10 +7584,10 @@
         <v>3954870000000</v>
       </c>
       <c r="F37">
-        <v>916580248937419.5</v>
+        <v>458290203033656.69</v>
       </c>
       <c r="G37">
-        <v>458339617468709.75</v>
+        <v>542391792858373.44</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.35">
@@ -7611,10 +7607,10 @@
         <v>3954870000000</v>
       </c>
       <c r="F38">
-        <v>916580248937419.5</v>
+        <v>458290203033656.69</v>
       </c>
       <c r="G38">
-        <v>458339617468709.75</v>
+        <v>542391792858373.44</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.35">
@@ -7634,10 +7630,10 @@
         <v>3954870000000</v>
       </c>
       <c r="F39">
-        <v>916580248937419.5</v>
+        <v>458290203033656.69</v>
       </c>
       <c r="G39">
-        <v>458339617468709.75</v>
+        <v>542391792858373.44</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.35">
@@ -7657,10 +7653,10 @@
         <v>3954870000000</v>
       </c>
       <c r="F40">
-        <v>916580248937419.5</v>
+        <v>458290203033656.69</v>
       </c>
       <c r="G40">
-        <v>458339617468709.75</v>
+        <v>542391792858373.44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>